<commit_message>
thinh pussh cho anh hieu lan 3
</commit_message>
<xml_diff>
--- a/INDRUINO_SOFT/IPQC_CHECKING_SYSTEM/bin/Debug/DBB.xlsx
+++ b/INDRUINO_SOFT/IPQC_CHECKING_SYSTEM/bin/Debug/DBB.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t xml:space="preserve">PartNumber</t>
   </si>
@@ -44,6 +44,9 @@
     <t xml:space="preserve">Result</t>
   </si>
   <si>
+    <t xml:space="preserve">Shown</t>
+  </si>
+  <si>
     <t xml:space="preserve">A2XM2610</t>
   </si>
   <si>
@@ -69,6 +72,21 @@
   </si>
   <si>
     <t xml:space="preserve">NG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repaired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSFDSF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy off sample</t>
   </si>
 </sst>
 </file>
@@ -104,8 +122,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+  <cellXfs count="33">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
@@ -171,72 +201,124 @@
         <v>8</v>
       </c>
       <c r="K2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2">
-        <v>43814.4326388889</v>
+        <v>43817.4326388889</v>
       </c>
       <c r="G3" s="4">
-        <v>43814.4340277778</v>
+        <v>43817.4340277778</v>
       </c>
       <c r="H3" s="6">
-        <v>43814.5652777778</v>
+        <v>43817.5652777778</v>
       </c>
       <c r="I3" s="8">
-        <v>43814.5298611111</v>
+        <v>43817.5298611111</v>
       </c>
       <c r="J3" s="10">
-        <v>43814.0847222222</v>
+        <v>43817.0847222222</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="L3"/>
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="12">
-        <v>43814.4743055556</v>
+        <v>43817.4743055556</v>
       </c>
       <c r="G4" s="14">
-        <v>43814.4756944444</v>
+        <v>43817.4756944444</v>
       </c>
       <c r="H4" s="16">
-        <v>43814.6069444444</v>
+        <v>43817.6069444444</v>
       </c>
       <c r="I4" s="18">
-        <v>43814.5715277778</v>
+        <v>43817.5715277778</v>
       </c>
       <c r="J4" s="20">
-        <v>43814.0840277778</v>
+        <v>43817.0840277778</v>
       </c>
       <c r="K4" t="s">
-        <v>18</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="L4"/>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5" s="22">
+        <v>43817.2791666667</v>
+      </c>
+      <c r="G5" s="24">
+        <v>43817.28125</v>
+      </c>
+      <c r="H5" s="26">
+        <v>43817.2833333333</v>
+      </c>
+      <c r="I5" s="28">
+        <v>43817.0020833333</v>
+      </c>
+      <c r="J5" s="30">
+        <v>43817.0041666667</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6" s="32">
+        <v>43817.28125</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>